<commit_message>
CAMBIOS Y MAS CAMBIOS
</commit_message>
<xml_diff>
--- a/web/archivos_generados/listadoAbagados2.xlsx
+++ b/web/archivos_generados/listadoAbagados2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>DETALLE</t>
   </si>
@@ -29,64 +29,16 @@
     <t>MONTO</t>
   </si>
   <si>
-    <t>jakldakljkljadlsd</t>
-  </si>
-  <si>
-    <t>01-02-2018</t>
+    <t xml:space="preserve">LIBRO Y VIAJE </t>
+  </si>
+  <si>
+    <t>16-02-2018</t>
   </si>
   <si>
     <t>INGRESO</t>
   </si>
   <si>
-    <t>$ 500.00</t>
-  </si>
-  <si>
-    <t>asdadasdasd</t>
-  </si>
-  <si>
-    <t>04-02-2018</t>
-  </si>
-  <si>
-    <t>$ 122.00</t>
-  </si>
-  <si>
-    <t>COBRO SERVICIOS</t>
-  </si>
-  <si>
-    <t>03-02-2018</t>
-  </si>
-  <si>
-    <t>$ 1200.00</t>
-  </si>
-  <si>
-    <t>06-02-2018</t>
-  </si>
-  <si>
-    <t>$ 1000.00</t>
-  </si>
-  <si>
-    <t>02-02-2018</t>
-  </si>
-  <si>
-    <t>$ 2150.00</t>
-  </si>
-  <si>
-    <t>09-02-2018</t>
-  </si>
-  <si>
-    <t>$ 800.00</t>
-  </si>
-  <si>
-    <t>$ 750.00</t>
-  </si>
-  <si>
-    <t>07-02-2018</t>
-  </si>
-  <si>
-    <t>$ 1500.00</t>
-  </si>
-  <si>
-    <t>$ 3350.00</t>
+    <t>$ 2500.00</t>
   </si>
 </sst>
 </file>
@@ -434,7 +386,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="D1" sqref="D1"/>
@@ -442,7 +394,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="11.711426" bestFit="true" customWidth="true" style="0"/>
@@ -474,118 +426,6 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>